<commit_message>
going great, updated flow, more in next push with README.md updated, just stamping progress today
</commit_message>
<xml_diff>
--- a/ebay-auto-listings.xlsx
+++ b/ebay-auto-listings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\dev\projects\ebay-posting-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB8C1A2B-A92E-4935-9C50-E4940C61E35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B18AF4A-E2E1-4B84-84FF-33012383587D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="5085" windowWidth="24330" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,11 @@
     <definedName name="CategoryNameNameFunction">[1]Categories!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
   <si>
     <t>*Action(SiteID=US|Country=US|Currency=USD|Version=1193)</t>
   </si>
@@ -379,15 +378,6 @@
     <t>William Shakespeare (edited by Harold Jenkins)</t>
   </si>
   <si>
-    <t>Methuen &amp; Co. Ltd., London, England / Methuen, Inc., New York, USA</t>
-  </si>
-  <si>
-    <t>1982</t>
-  </si>
-  <si>
-    <t>First Edition, First Printing of the Harold Jenkins Arden edition</t>
-  </si>
-  <si>
     <t>The Works of Christopher Marlowe</t>
   </si>
   <si>
@@ -417,15 +407,6 @@
   </si>
   <si>
     <t>Christopher Marlowe (edited by C. F. Tucker Brooke)</t>
-  </si>
-  <si>
-    <t>Oxford at the Clarendon Press (Oxford University Press), Oxford, United Kingdom</t>
-  </si>
-  <si>
-    <t>1969</t>
-  </si>
-  <si>
-    <t>1969 Reprint (11th impression of the 1910 Oxford text)</t>
   </si>
   <si>
     <t>Generated</t>
@@ -931,11 +912,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AY21" sqref="AY21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="18" width="14" customWidth="1"/>
+    <col min="36" max="36" width="31.5703125" customWidth="1"/>
+    <col min="37" max="37" width="33.5703125" customWidth="1"/>
+    <col min="38" max="38" width="32.140625" customWidth="1"/>
+    <col min="39" max="39" width="34.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1299,15 +1287,6 @@
       <c r="AO3" t="s">
         <v>97</v>
       </c>
-      <c r="AQ3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="4" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1320,7 +1299,7 @@
         <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -1335,7 +1314,7 @@
         <v>88</v>
       </c>
       <c r="P4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="Q4" t="s">
         <v>90</v>
@@ -1356,22 +1335,13 @@
         <v>95</v>
       </c>
       <c r="AM4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AN4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AO4" t="s">
         <v>97</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1397,6 +1367,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1410,10 +1381,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
has gotten worse since last commit, started new branch diff-pipeline-approach to try and repair
</commit_message>
<xml_diff>
--- a/ebay-auto-listings.xlsx
+++ b/ebay-auto-listings.xlsx
@@ -8,26 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\dev\projects\ebay-posting-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B18AF4A-E2E1-4B84-84FF-33012383587D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4DE39A-AAF2-417E-8976-A27572746BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="24285" windowHeight="9615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
     <sheet name="INFO" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="CategoryNameNameFunction">[1]Categories!$A$2:$A$3</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>*Action(SiteID=US|Country=US|Currency=USD|Version=1193)</t>
   </si>
@@ -278,141 +272,10 @@
     <t>Responsible Person 1 ContactURL</t>
   </si>
   <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>261186</t>
-  </si>
-  <si>
-    <t>/Books &amp; Magazines/Books</t>
-  </si>
-  <si>
-    <t>True to the Old Flag: A Tale of the American War of Independence</t>
-  </si>
-  <si>
-    <t>https://keith-ebay-images.s3.us-east-2.amazonaws.com/IMG_4929.JPG</t>
-  </si>
-  <si>
-    <t>5000-Good</t>
-  </si>
-  <si>
-    <t>G. A. Henty's classic adventure plunges readers into the tumult of the American Revolution, following a young loyalist who struggles to remain faithful to King and country amid the growing conflict. This handsome PrestonSpeed Heirloom edition offers sturdy library-quality binding, crisp type, and Gordoun Browne's original illustrations-perfect for collectors, homeschoolers, or fans of historical fiction.
-Condition Notes:
-Near Fine: blue cloth bright and clean; gilt titles sharp; square, tight binding; no writing or marks observed; minimal shelf rub to extremities, no jacket as issued.
-Collector Details:
-Bibliographic Details
-- Author: G. A. Henty (1832-1902)
-- Title: True to the Old Flag: A Tale of the American War of Independence
-- Illustrator: Gordon Browne (frontispiece &amp; text illustrations reproduced)
-- Publisher / Place: PrestonSpeed Publications, 51 Ridge Road, Mill Hall, Pennsylvania, USA
-- Year: 2002 (copyright (c) 2001 by PrestonSpeed; printer's line dated November 2002)
-- Edition / Printing: Heirloom Hardcover Edition, first PrestonSpeed printing; ISBN 1-888715-14-2
-- Format: Octavo (8vo) hardcover; xiv + 384 pp. (publisher's pagination)
-- Binding Details: Navy blue cloth over boards; gilt ruled borders, stars &amp; compass rose device to upper board; gilt titling to spine; smooth navy endpapers
-- Dust Jacket: None issued with Heirloom binding
-- Notable Points: High-quality acid-free paper and reinforced binding for longevity; unabridged text of the 1885 first edition; part of PrestonSpeed's Henty reprint series
-- Language: English
-Condition (conservative, ABAA-style)
-- Boards/Spine: Cloth fresh, only the lightest rub at one spine corner.
-- Pages/Textblock: Bright, clean, unmarked; no foxing or edge tears.
-- Hinges/Binding: Tight, square, appears unread.
-- Edges: Clean with faint shelf dust.
-- Overall grade: Near Fine.</t>
-  </si>
-  <si>
-    <t>FixedPrice</t>
-  </si>
-  <si>
-    <t>GTC</t>
-  </si>
-  <si>
-    <t>Newfields, NH</t>
-  </si>
-  <si>
-    <t>USPS Media Mail</t>
-  </si>
-  <si>
-    <t>Returns allowed within 30 days</t>
-  </si>
-  <si>
-    <t>Immediate payment managed via eBay</t>
-  </si>
-  <si>
-    <t>G. A. Henty</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Hamlet (The Arden Shakespeare)</t>
-  </si>
-  <si>
-    <t>Sought-after scholarly Arden text of Shakespeare's greatest tragedy, meticulously edited and annotated by Harold Jenkins. Ideal for collectors of Shakespeareana or students wanting the definitive modern critical edition, complete with extensive introduction, textual apparatus, and notes. Scarce 1982 first printing in original dust-jacket.
-Condition Notes:
-Dust-jacket rubbed, edge-worn with small tears, chips and a damp-stain to lower front panel; spine lightly sunned. Blue cloth boards clean; corners sharp. Text block bright, unmarked, firm binding. Overall a solid Very Good book in Good jacket.
-Collector Details:
-Bibliographic Details
-- Author: William Shakespeare
-- Editor: Harold Jenkins (Arden general editor)
-- Title: Hamlet (The Arden Edition of the Works of William Shakespeare)
-- Publisher / Place: Methuen &amp; Co. Ltd., 11 New Fetter Lane, London EC4P 4EE; in association with Methuen, Inc., 733 Third Avenue, New York, NY 10017
-- Year: 1982
-- Edition / Printing: First Edition, First Printing of this Jenkins-edited text (copyright page states "first published in 1982" with no later impressions noted)
-- Series: The Arden Shakespeare (2nd series)
-- ISBN: 0-416-17910-X (hardback); 0-416-17920-7 (paperback listed)
-- Format: Large 8vo hardcover; xxviii + 507 pp. (including extensive introduction, commentary, textual notes, appendices, bibliography, index)
-- Binding Details: Publisher's blue cloth; gilt spine lettering; plain endpapers; sewn signatures
-- Dust Jacket: Cream printed jacket with decorative border; priced; series list to rear panel
-- Notable Points: Highly regarded critical edition; comprehensive textual discussion; cornerstone for Shakespeare scholars
-- Language: English
-Condition (conservative, ABAA-style)
-- Boards/Spine: Clean cloth; minimal rubbing at extremities; gilt bright; slight lean.
-- Pages/Textblock: Fresh, crisp pages; no marks or underlining observed; edges lightly toned.
-- Illustrations/Facsimiles: Contains facsimile title pages and textual figures; all present.
-- Hinges/Binding: Solid, square, no cracking.
-- Edges: Very light dust-soil top edge.
-- Dust Jacket: Good only-overall toning, surface scuffs, several short closed tears, small chip at crown, damp stain along lower front joint; now in removable archival mylar.
-- Overall grade: Very Good book in Good jacket.</t>
-  </si>
-  <si>
-    <t>William Shakespeare (edited by Harold Jenkins)</t>
-  </si>
-  <si>
-    <t>The Works of Christopher Marlowe</t>
-  </si>
-  <si>
-    <t>Handsome Oxford re-issue of Christopher Marlowe's complete works, meticulously edited by scholar C. F. Tucker Brooke. Includes the full texts of Doctor Faustus, Tamburlaine, The Jew of Malta, and all the poems with scholarly introduction and notes. A solid mid-century hardcover in the original dust-jacket-ideal for students, collectors of Elizabethan drama, or anyone who wants a reliable reading copy of England's fiery Renaissance playwright.
-Condition Notes:
-Dust-jacket toned, edge-worn with small chips/tears at spine ends &amp; corners; a few surface spots. Green cloth boards clean, bright gilt to spine. Text clean and unmarked save for small pencil shelf mark on title. Binding tight. Very Good book in Good jacket.
-Collector Details:
-- Bibliographic Details
-  Author: Christopher Marlowe
-  Editor: C. F. Tucker Brooke (B.Litt. Oxon.; later Professor of English, Yale University)
-  Title: The Works of Christopher Marlowe
-  Publisher / Place: Oxford at the Clarendon Press (Oxford University Press), Oxford
-  Year: 1969 reprint (first published 1910; subsequent reprints 1925, 1929, 1941, 1946, 1953, 1957, 1962, 1964, 1966, 1969)
-  Edition / Printing: Eleventh impression, July 1969 (print code 7/69 on jacket rear panel)
-  Format: Crown 8vo hardcover; approx. 8.75 × 5.5 in.; xv + 468 pp. (pagination not fully verified)
-  Binding Details: Original dark green cloth; gilt titling to spine; plain endpapers
-  Dust Jacket: Cream jacket printed red; Oxford device to front panel &amp; spine; price-clipped
-  Notable Points: Standard scholarly text of Marlowe for much of the 20th C.; includes textual notes and Brooke's critical introduction.
-  Language: English
-  Condition (conservative, ABAA-style)
-  - Boards/Spine: Cloth bright; mild rubbing to extremities.
-  - Pages/Textblock: Clean; no writing or highlighting; mild toning at edges.
-  - Hinges/Binding: Square and sound; no cracking.
-  - Edges: Light age-toning, faint dust-soil top edge.
-  - Dust Jacket: Toned; shallow chips at crown/foot, corners; short closed tears, small surface spots; now in removable archival sleeve.
-  Overall grade: Very Good book in Good jacket.</t>
-  </si>
-  <si>
-    <t>Christopher Marlowe (edited by C. F. Tucker Brooke)</t>
-  </si>
-  <si>
     <t>Generated</t>
   </si>
   <si>
-    <t>2025-10-13T20:16:44</t>
+    <t>2025-10-14T16:59:31</t>
   </si>
 </sst>
 </file>
@@ -454,129 +317,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF5965"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD0CECE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF5965"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD0CECE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -587,42 +328,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="GENERAL INSTRUCTIONS"/>
-      <sheetName val="Listings"/>
-      <sheetName val="Categories"/>
-      <sheetName val="ListingStaticData"/>
-      <sheetName val="BusinessPolicy"/>
-      <sheetName val="Aspects"/>
-      <sheetName val="ConditionDescriptors"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>/Books &amp; Magazines/Books</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>/Books &amp; Magazines/Antiquarian &amp; Collectible</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -910,20 +615,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE4"/>
+  <dimension ref="A1:CE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AY21" sqref="AY21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="18" width="14" customWidth="1"/>
-    <col min="36" max="36" width="31.5703125" customWidth="1"/>
-    <col min="37" max="37" width="33.5703125" customWidth="1"/>
-    <col min="38" max="38" width="32.140625" customWidth="1"/>
-    <col min="39" max="39" width="34.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1176,198 +874,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P2" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>90</v>
-      </c>
-      <c r="R2" t="s">
-        <v>91</v>
-      </c>
-      <c r="X2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K3">
-        <v>5</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>87</v>
-      </c>
-      <c r="O3" t="s">
-        <v>88</v>
-      </c>
-      <c r="P3" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>90</v>
-      </c>
-      <c r="R3" t="s">
-        <v>91</v>
-      </c>
-      <c r="X3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" t="s">
-        <v>101</v>
-      </c>
-      <c r="K4">
-        <v>5</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>87</v>
-      </c>
-      <c r="O4" t="s">
-        <v>88</v>
-      </c>
-      <c r="P4" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>90</v>
-      </c>
-      <c r="R4" t="s">
-        <v>91</v>
-      </c>
-      <c r="X4" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>97</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="AJ2">
-    <cfRule type="expression" dxfId="4" priority="11" stopIfTrue="1">
-      <formula>AND(NOT(ISBLANK(A2)), OR(NOT(ISBLANK(Y2)), NOT(ISBLANK(Z2)), NOT(ISBLANK(AE2))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="12">
-      <formula>NOT(ISBLANK(A2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ2:AK2">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
-      <formula>NOT(ISBLANK(AJ2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK2">
-    <cfRule type="expression" dxfId="1" priority="13" stopIfTrue="1">
-      <formula>AND(NOT(ISBLANK(A2)), OR(NOT(ISBLANK(AF2)), NOT(ISBLANK(AG2)), NOT(ISBLANK(AI2))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
-      <formula>NOT(ISBLANK(A2))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1381,10 +889,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename...py not working, switching back to main
</commit_message>
<xml_diff>
--- a/ebay-auto-listings.xlsx
+++ b/ebay-auto-listings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\dev\projects\ebay-posting-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB8C1A2B-A92E-4935-9C50-E4940C61E35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D7B233-2381-4680-9E1D-660C327FE439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="5085" windowWidth="24330" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="24285" windowHeight="9615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,25 @@
   <definedNames>
     <definedName name="CategoryNameNameFunction">[1]Categories!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
   <si>
     <t>*Action(SiteID=US|Country=US|Currency=USD|Version=1193)</t>
   </si>
@@ -288,39 +300,9 @@
     <t>/Books &amp; Magazines/Books</t>
   </si>
   <si>
-    <t>True to the Old Flag: A Tale of the American War of Independence</t>
-  </si>
-  <si>
-    <t>https://keith-ebay-images.s3.us-east-2.amazonaws.com/IMG_4929.JPG</t>
-  </si>
-  <si>
     <t>5000-Good</t>
   </si>
   <si>
-    <t>G. A. Henty's classic adventure plunges readers into the tumult of the American Revolution, following a young loyalist who struggles to remain faithful to King and country amid the growing conflict. This handsome PrestonSpeed Heirloom edition offers sturdy library-quality binding, crisp type, and Gordoun Browne's original illustrations-perfect for collectors, homeschoolers, or fans of historical fiction.
-Condition Notes:
-Near Fine: blue cloth bright and clean; gilt titles sharp; square, tight binding; no writing or marks observed; minimal shelf rub to extremities, no jacket as issued.
-Collector Details:
-Bibliographic Details
-- Author: G. A. Henty (1832-1902)
-- Title: True to the Old Flag: A Tale of the American War of Independence
-- Illustrator: Gordon Browne (frontispiece &amp; text illustrations reproduced)
-- Publisher / Place: PrestonSpeed Publications, 51 Ridge Road, Mill Hall, Pennsylvania, USA
-- Year: 2002 (copyright (c) 2001 by PrestonSpeed; printer's line dated November 2002)
-- Edition / Printing: Heirloom Hardcover Edition, first PrestonSpeed printing; ISBN 1-888715-14-2
-- Format: Octavo (8vo) hardcover; xiv + 384 pp. (publisher's pagination)
-- Binding Details: Navy blue cloth over boards; gilt ruled borders, stars &amp; compass rose device to upper board; gilt titling to spine; smooth navy endpapers
-- Dust Jacket: None issued with Heirloom binding
-- Notable Points: High-quality acid-free paper and reinforced binding for longevity; unabridged text of the 1885 first edition; part of PrestonSpeed's Henty reprint series
-- Language: English
-Condition (conservative, ABAA-style)
-- Boards/Spine: Cloth fresh, only the lightest rub at one spine corner.
-- Pages/Textblock: Bright, clean, unmarked; no foxing or edge tears.
-- Hinges/Binding: Tight, square, appears unread.
-- Edges: Clean with faint shelf dust.
-- Overall grade: Near Fine.</t>
-  </si>
-  <si>
     <t>FixedPrice</t>
   </si>
   <si>
@@ -339,99 +321,74 @@
     <t>Immediate payment managed via eBay</t>
   </si>
   <si>
-    <t>G. A. Henty</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
-    <t>Hamlet (The Arden Shakespeare)</t>
-  </si>
-  <si>
-    <t>Sought-after scholarly Arden text of Shakespeare's greatest tragedy, meticulously edited and annotated by Harold Jenkins. Ideal for collectors of Shakespeareana or students wanting the definitive modern critical edition, complete with extensive introduction, textual apparatus, and notes. Scarce 1982 first printing in original dust-jacket.
-Condition Notes:
-Dust-jacket rubbed, edge-worn with small tears, chips and a damp-stain to lower front panel; spine lightly sunned. Blue cloth boards clean; corners sharp. Text block bright, unmarked, firm binding. Overall a solid Very Good book in Good jacket.
+    <t>The Two Gentlemen of Verona (The Arden Shakespeare)</t>
+  </si>
+  <si>
+    <t>Condition Notes:
+Very Good in Good+ jacket: blue cloth boards bright; binding square and tight; pages clean with only faint toning to edges. Jacket retains colour, light edge-rubs, small chip at head of spine and faint splash mark to lower rear panel, now in removable archival sleeve.
 Collector Details:
 Bibliographic Details
 - Author: William Shakespeare
-- Editor: Harold Jenkins (Arden general editor)
-- Title: Hamlet (The Arden Edition of the Works of William Shakespeare)
-- Publisher / Place: Methuen &amp; Co. Ltd., 11 New Fetter Lane, London EC4P 4EE; in association with Methuen, Inc., 733 Third Avenue, New York, NY 10017
-- Year: 1982
-- Edition / Printing: First Edition, First Printing of this Jenkins-edited text (copyright page states "first published in 1982" with no later impressions noted)
-- Series: The Arden Shakespeare (2nd series)
-- ISBN: 0-416-17910-X (hardback); 0-416-17920-7 (paperback listed)
-- Format: Large 8vo hardcover; xxviii + 507 pp. (including extensive introduction, commentary, textual notes, appendices, bibliography, index)
-- Binding Details: Publisher's blue cloth; gilt spine lettering; plain endpapers; sewn signatures
-- Dust Jacket: Cream printed jacket with decorative border; priced; series list to rear panel
-- Notable Points: Highly regarded critical edition; comprehensive textual discussion; cornerstone for Shakespeare scholars
+- Title: The Two Gentlemen of Verona
+- Editor: Clifford Leech (Arden Second Series)
+- Publisher / Place: Methuen &amp; Co. Ltd., London
+- Year: 1969
+- Edition / Printing: First printing of the completely revised &amp; reset edition (first thus for Leech text; previous Arden issue 1906 by Warwick Bond)
+- Format: Crown 8vo hardcover; li + 188 pp. including Introduction, Text, Commentary &amp; Index
+- Binding Details: Original blue cloth; gilt spine lettering; publisher's blind colophon to upper board
+- Dust Jacket: Printed teal/white jacket with decorative border; priced; now protected in Mylar
+- Notable Points: Includes comprehensive introduction on sources, date, stage history; full textual notes; SBN 416 47490 X
 - Language: English
 Condition (conservative, ABAA-style)
-- Boards/Spine: Clean cloth; minimal rubbing at extremities; gilt bright; slight lean.
-- Pages/Textblock: Fresh, crisp pages; no marks or underlining observed; edges lightly toned.
-- Illustrations/Facsimiles: Contains facsimile title pages and textual figures; all present.
-- Hinges/Binding: Solid, square, no cracking.
-- Edges: Very light dust-soil top edge.
-- Dust Jacket: Good only-overall toning, surface scuffs, several short closed tears, small chip at crown, damp stain along lower front joint; now in removable archival mylar.
-- Overall grade: Very Good book in Good jacket.</t>
-  </si>
-  <si>
-    <t>William Shakespeare (edited by Harold Jenkins)</t>
-  </si>
-  <si>
-    <t>Methuen &amp; Co. Ltd., London, England / Methuen, Inc., New York, USA</t>
-  </si>
-  <si>
-    <t>1982</t>
-  </si>
-  <si>
-    <t>First Edition, First Printing of the Harold Jenkins Arden edition</t>
-  </si>
-  <si>
-    <t>The Works of Christopher Marlowe</t>
-  </si>
-  <si>
-    <t>Handsome Oxford re-issue of Christopher Marlowe's complete works, meticulously edited by scholar C. F. Tucker Brooke. Includes the full texts of Doctor Faustus, Tamburlaine, The Jew of Malta, and all the poems with scholarly introduction and notes. A solid mid-century hardcover in the original dust-jacket-ideal for students, collectors of Elizabethan drama, or anyone who wants a reliable reading copy of England's fiery Renaissance playwright.
-Condition Notes:
-Dust-jacket toned, edge-worn with small chips/tears at spine ends &amp; corners; a few surface spots. Green cloth boards clean, bright gilt to spine. Text clean and unmarked save for small pencil shelf mark on title. Binding tight. Very Good book in Good jacket.
+- Boards/Spine: Clean cloth, minor rubbing to extremities, bright gilt
+- Pages/Textblock: Creamy pages, firm; no writing or marks noted
+- Hinges/Binding: Tight, square; no cracking
+- Edges: Very slight dusting to top edge
+- Dust Jacket: Edge-wear with short closed tears, nick at spine crown, faint rear panel staining; colors strong, unclipped
+- Overall grade: Very Good book / Good+ jacket</t>
+  </si>
+  <si>
+    <t>William Shakespeare</t>
+  </si>
+  <si>
+    <t>The Sacred Tree: Being the Second Part of ‘The Tale of Genji'</t>
+  </si>
+  <si>
+    <t>Collector Details:
+['Bibliographic Details', 'Author: Lady Murasaki (Murasaki Shikibu)', 'Translator: Arthur Waley', 'Title: The Sacred Tree: Being the Second Part of ‘The Tale of Genji'', 'Publisher / Place: Houghton Mifflin Company, Boston &amp; New York (printed at The Riverside Press, Cambridge)', 'Year: 1926', 'Edition / Printing: First American Edition, First Printing', 'Series / Universe: Arthur Waley's six-volume Tale of Genji translation (vol. II)', 'Format: Crown 8vo hardcover; approx. xx + 287 pp.', 'Binding Details: Quarter green cloth; Japanese geometric/floral patterned paper over boards; paper spine label printed in black; top edge green; deckle fore-edge', 'Dust Jacket: No jacket issued with U.S. trade edition; originally supplied in a plain card slipcase (not present)', 'Notable Points: Early English-language access to a cornerstone of classical Japanese literature; highly regarded Waley translation', 'Language: English (translated from classical Japanese)', 'Condition (conservative, ABAA-style)', 'Boards/Spine: Patterned boards bright; light rubbing to edges; corners worn through at tips; cloth spine clean with minor fray at crown/foot; spine label toned but legible.', 'Pages/Textblock: Uniform creamy toning; no marking or foxing observed; top edge tint somewhat faded.', 'Hinges/Binding: Firm and square; no loose gatherings.', 'Edges: Deckle fore-edge rough-cut as issued; mild dust-soil.', 'Overall grade: Very Good- (well-kept copy, minor shelf wear, no restoration).']</t>
+  </si>
+  <si>
+    <t>Lady Murasaki (Murasaki Shikibu); translated by Arthur Waley</t>
+  </si>
+  <si>
+    <t>Pearl; Sir Gawain and the Green Knight</t>
+  </si>
+  <si>
+    <t>Condition Notes:
+Good+. Clean brown cloth a little rubbed with a surface scratch to upper board, mild fray to spine foot &amp; a corner; gilt spine titling bright. Page edges evenly toned, one small smudge to lower edge. EL endpapers show owner's pencilled &amp; inked notes. Tight, square binding; text clean with only scattered faint handling.
 Collector Details:
-- Bibliographic Details
-  Author: Christopher Marlowe
-  Editor: C. F. Tucker Brooke (B.Litt. Oxon.; later Professor of English, Yale University)
-  Title: The Works of Christopher Marlowe
-  Publisher / Place: Oxford at the Clarendon Press (Oxford University Press), Oxford
-  Year: 1969 reprint (first published 1910; subsequent reprints 1925, 1929, 1941, 1946, 1953, 1957, 1962, 1964, 1966, 1969)
-  Edition / Printing: Eleventh impression, July 1969 (print code 7/69 on jacket rear panel)
-  Format: Crown 8vo hardcover; approx. 8.75 × 5.5 in.; xv + 468 pp. (pagination not fully verified)
-  Binding Details: Original dark green cloth; gilt titling to spine; plain endpapers
-  Dust Jacket: Cream jacket printed red; Oxford device to front panel &amp; spine; price-clipped
-  Notable Points: Standard scholarly text of Marlowe for much of the 20th C.; includes textual notes and Brooke's critical introduction.
-  Language: English
-  Condition (conservative, ABAA-style)
-  - Boards/Spine: Cloth bright; mild rubbing to extremities.
-  - Pages/Textblock: Clean; no writing or highlighting; mild toning at edges.
-  - Hinges/Binding: Square and sound; no cracking.
-  - Edges: Light age-toning, faint dust-soil top edge.
-  - Dust Jacket: Toned; shallow chips at crown/foot, corners; short closed tears, small surface spots; now in removable archival sleeve.
-  Overall grade: Very Good book in Good jacket.</t>
-  </si>
-  <si>
-    <t>Christopher Marlowe (edited by C. F. Tucker Brooke)</t>
-  </si>
-  <si>
-    <t>Oxford at the Clarendon Press (Oxford University Press), Oxford, United Kingdom</t>
-  </si>
-  <si>
-    <t>1969</t>
-  </si>
-  <si>
-    <t>1969 Reprint (11th impression of the 1910 Oxford text)</t>
+['Bibliographic Details', 'Author: Anonymous (‘Pearl' / ‘Gawain' Poet); Editor &amp; Introduction: A. C. Cawley', 'Title: Pearl; Sir Gawain and the Green Knight', 'Publisher / Place: J. M. Dent &amp; Sons Ltd., Aldine House, Bedford St., London | Co-issue: E. P. Dutton &amp; Co., New York', 'Year: 1966 (copyright 1962; statement: ‘Last reprinted 1966')', 'Edition / Printing: Everyman's Library No. 346, 1966 Reprint', 'Format: Crown 8vo hardcover; approx. xxxii + 204 pp.', 'Binding Details: Original brown cloth; double gilt rules at crown; gilt titling &amp; EL script monogram to spine; EL anchor-monogram patterned endpapers', 'Dust Jacket: Not present (often lost)', 'Notable Points: Full Middle English text with scholarly apparatus; glossary, textual notes, bibliographical check-list', 'Language: English (Middle English text with modern English notes)', 'Condition (conservative, ABAA-style)', 'Boards/Spine: Light rubbing; surface scratch to upper board; mild corner &amp; spine-end wear; gilt bright.', 'Pages/Textblock: Clean, evenly toned stock; a few faint handling marks; no underlining in text.', 'Endpapers: EL pattern; previous owner's ink annotations on front &amp; rear pastedowns.', 'Hinges/Binding: Firm and square; no loose leaves.', 'Edges: Toned; one small spot to lower edge.', 'Overall grade: Good+ (solid reading / reference copy in original cloth).']</t>
+  </si>
+  <si>
+    <t>Anonymous (The Pearl / Gawain Poet); edited with introduction by A. C. Cawley, M.A., Ph.D.</t>
   </si>
   <si>
     <t>Generated</t>
   </si>
   <si>
     <t>2025-10-13T20:16:44</t>
+  </si>
+  <si>
+    <t>https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-06.jpg</t>
+  </si>
+  <si>
+    <t>https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-06.jpg</t>
+  </si>
+  <si>
+    <t>https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-06.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-07.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-08.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-09.jpg</t>
   </si>
 </sst>
 </file>
@@ -467,135 +424,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF5965"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD0CECE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF5965"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD0CECE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -929,13 +767,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE4"/>
+  <dimension ref="A1:CE9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="14" width="1.140625" customWidth="1"/>
+    <col min="16" max="16" width="166.85546875" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -983,7 +825,7 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">
@@ -1188,7 +1030,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" ht="360" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -1199,52 +1041,52 @@
         <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q2" t="s">
         <v>87</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>88</v>
       </c>
-      <c r="P2" t="s">
+      <c r="X2" t="s">
         <v>89</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="AJ2" t="s">
         <v>90</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AK2" t="s">
         <v>91</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AL2" t="s">
         <v>92</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>95</v>
       </c>
       <c r="AM2" t="s">
         <v>96</v>
       </c>
       <c r="AN2" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="AO2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -1255,61 +1097,52 @@
         <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3" t="s">
+        <v>106</v>
+      </c>
+      <c r="O3" t="s">
+        <v>86</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q3" t="s">
         <v>87</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>88</v>
       </c>
-      <c r="P3" t="s">
+      <c r="X3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM3" t="s">
         <v>99</v>
       </c>
-      <c r="Q3" t="s">
-        <v>90</v>
-      </c>
-      <c r="R3" t="s">
-        <v>91</v>
-      </c>
-      <c r="X3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ3" t="s">
+      <c r="AN3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AO3" t="s">
         <v>93</v>
       </c>
-      <c r="AK3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>103</v>
-      </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:83" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1320,82 +1153,58 @@
         <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K4">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
       <c r="M4" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" t="s">
+        <v>86</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q4" t="s">
         <v>87</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>88</v>
       </c>
-      <c r="P4" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="X4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>90</v>
       </c>
-      <c r="R4" t="s">
+      <c r="AK4" t="s">
         <v>91</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AL4" t="s">
         <v>92</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AM4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO4" t="s">
         <v>93</v>
       </c>
-      <c r="AK4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>106</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>109</v>
+    </row>
+    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="AZ9">
+        <f>LEN(AZ4)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AJ2">
-    <cfRule type="expression" dxfId="4" priority="11" stopIfTrue="1">
-      <formula>AND(NOT(ISBLANK(A2)), OR(NOT(ISBLANK(Y2)), NOT(ISBLANK(Z2)), NOT(ISBLANK(AE2))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="12">
-      <formula>NOT(ISBLANK(A2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ2:AK2">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
-      <formula>NOT(ISBLANK(AJ2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK2">
-    <cfRule type="expression" dxfId="1" priority="13" stopIfTrue="1">
-      <formula>AND(NOT(ISBLANK(A2)), OR(NOT(ISBLANK(AF2)), NOT(ISBLANK(AG2)), NOT(ISBLANK(AI2))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
-      <formula>NOT(ISBLANK(A2))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1410,10 +1219,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
good progress, main will die soon :)
</commit_message>
<xml_diff>
--- a/ebay-auto-listings.xlsx
+++ b/ebay-auto-listings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\dev\projects\ebay-posting-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D7B233-2381-4680-9E1D-660C327FE439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B5E34F-3BF2-4151-BC2B-93FD96954995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="0" windowWidth="24285" windowHeight="9615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="690" windowWidth="24285" windowHeight="9615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>*Action(SiteID=US|Country=US|Currency=USD|Version=1193)</t>
   </si>
@@ -291,104 +291,10 @@
     <t>Responsible Person 1 ContactURL</t>
   </si>
   <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>261186</t>
-  </si>
-  <si>
-    <t>/Books &amp; Magazines/Books</t>
-  </si>
-  <si>
-    <t>5000-Good</t>
-  </si>
-  <si>
-    <t>FixedPrice</t>
-  </si>
-  <si>
-    <t>GTC</t>
-  </si>
-  <si>
-    <t>Newfields, NH</t>
-  </si>
-  <si>
-    <t>USPS Media Mail</t>
-  </si>
-  <si>
-    <t>Returns allowed within 30 days</t>
-  </si>
-  <si>
-    <t>Immediate payment managed via eBay</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>The Two Gentlemen of Verona (The Arden Shakespeare)</t>
-  </si>
-  <si>
-    <t>Condition Notes:
-Very Good in Good+ jacket: blue cloth boards bright; binding square and tight; pages clean with only faint toning to edges. Jacket retains colour, light edge-rubs, small chip at head of spine and faint splash mark to lower rear panel, now in removable archival sleeve.
-Collector Details:
-Bibliographic Details
-- Author: William Shakespeare
-- Title: The Two Gentlemen of Verona
-- Editor: Clifford Leech (Arden Second Series)
-- Publisher / Place: Methuen &amp; Co. Ltd., London
-- Year: 1969
-- Edition / Printing: First printing of the completely revised &amp; reset edition (first thus for Leech text; previous Arden issue 1906 by Warwick Bond)
-- Format: Crown 8vo hardcover; li + 188 pp. including Introduction, Text, Commentary &amp; Index
-- Binding Details: Original blue cloth; gilt spine lettering; publisher's blind colophon to upper board
-- Dust Jacket: Printed teal/white jacket with decorative border; priced; now protected in Mylar
-- Notable Points: Includes comprehensive introduction on sources, date, stage history; full textual notes; SBN 416 47490 X
-- Language: English
-Condition (conservative, ABAA-style)
-- Boards/Spine: Clean cloth, minor rubbing to extremities, bright gilt
-- Pages/Textblock: Creamy pages, firm; no writing or marks noted
-- Hinges/Binding: Tight, square; no cracking
-- Edges: Very slight dusting to top edge
-- Dust Jacket: Edge-wear with short closed tears, nick at spine crown, faint rear panel staining; colors strong, unclipped
-- Overall grade: Very Good book / Good+ jacket</t>
-  </si>
-  <si>
-    <t>William Shakespeare</t>
-  </si>
-  <si>
-    <t>The Sacred Tree: Being the Second Part of ‘The Tale of Genji'</t>
-  </si>
-  <si>
-    <t>Collector Details:
-['Bibliographic Details', 'Author: Lady Murasaki (Murasaki Shikibu)', 'Translator: Arthur Waley', 'Title: The Sacred Tree: Being the Second Part of ‘The Tale of Genji'', 'Publisher / Place: Houghton Mifflin Company, Boston &amp; New York (printed at The Riverside Press, Cambridge)', 'Year: 1926', 'Edition / Printing: First American Edition, First Printing', 'Series / Universe: Arthur Waley's six-volume Tale of Genji translation (vol. II)', 'Format: Crown 8vo hardcover; approx. xx + 287 pp.', 'Binding Details: Quarter green cloth; Japanese geometric/floral patterned paper over boards; paper spine label printed in black; top edge green; deckle fore-edge', 'Dust Jacket: No jacket issued with U.S. trade edition; originally supplied in a plain card slipcase (not present)', 'Notable Points: Early English-language access to a cornerstone of classical Japanese literature; highly regarded Waley translation', 'Language: English (translated from classical Japanese)', 'Condition (conservative, ABAA-style)', 'Boards/Spine: Patterned boards bright; light rubbing to edges; corners worn through at tips; cloth spine clean with minor fray at crown/foot; spine label toned but legible.', 'Pages/Textblock: Uniform creamy toning; no marking or foxing observed; top edge tint somewhat faded.', 'Hinges/Binding: Firm and square; no loose gatherings.', 'Edges: Deckle fore-edge rough-cut as issued; mild dust-soil.', 'Overall grade: Very Good- (well-kept copy, minor shelf wear, no restoration).']</t>
-  </si>
-  <si>
-    <t>Lady Murasaki (Murasaki Shikibu); translated by Arthur Waley</t>
-  </si>
-  <si>
-    <t>Pearl; Sir Gawain and the Green Knight</t>
-  </si>
-  <si>
-    <t>Condition Notes:
-Good+. Clean brown cloth a little rubbed with a surface scratch to upper board, mild fray to spine foot &amp; a corner; gilt spine titling bright. Page edges evenly toned, one small smudge to lower edge. EL endpapers show owner's pencilled &amp; inked notes. Tight, square binding; text clean with only scattered faint handling.
-Collector Details:
-['Bibliographic Details', 'Author: Anonymous (‘Pearl' / ‘Gawain' Poet); Editor &amp; Introduction: A. C. Cawley', 'Title: Pearl; Sir Gawain and the Green Knight', 'Publisher / Place: J. M. Dent &amp; Sons Ltd., Aldine House, Bedford St., London | Co-issue: E. P. Dutton &amp; Co., New York', 'Year: 1966 (copyright 1962; statement: ‘Last reprinted 1966')', 'Edition / Printing: Everyman's Library No. 346, 1966 Reprint', 'Format: Crown 8vo hardcover; approx. xxxii + 204 pp.', 'Binding Details: Original brown cloth; double gilt rules at crown; gilt titling &amp; EL script monogram to spine; EL anchor-monogram patterned endpapers', 'Dust Jacket: Not present (often lost)', 'Notable Points: Full Middle English text with scholarly apparatus; glossary, textual notes, bibliographical check-list', 'Language: English (Middle English text with modern English notes)', 'Condition (conservative, ABAA-style)', 'Boards/Spine: Light rubbing; surface scratch to upper board; mild corner &amp; spine-end wear; gilt bright.', 'Pages/Textblock: Clean, evenly toned stock; a few faint handling marks; no underlining in text.', 'Endpapers: EL pattern; previous owner's ink annotations on front &amp; rear pastedowns.', 'Hinges/Binding: Firm and square; no loose leaves.', 'Edges: Toned; one small spot to lower edge.', 'Overall grade: Good+ (solid reading / reference copy in original cloth).']</t>
-  </si>
-  <si>
-    <t>Anonymous (The Pearl / Gawain Poet); edited with introduction by A. C. Cawley, M.A., Ph.D.</t>
-  </si>
-  <si>
     <t>Generated</t>
   </si>
   <si>
     <t>2025-10-13T20:16:44</t>
-  </si>
-  <si>
-    <t>https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/arden-shakespeare-two-gent-verona-2/arden-shakespeare-two-gent-verona-2-06.jpg</t>
-  </si>
-  <si>
-    <t>https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/murasaki-cayley-sacred-tree-2/murasaki-cayley-sacred-tree-2-06.jpg</t>
-  </si>
-  <si>
-    <t>https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-01.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-02.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-03.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-04.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-05.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-06.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-07.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-08.jpg | https://keith-ebay-images.s3.amazonaws.com/books/pearl-gawain-green-knight-2/pearl-gawain-green-knight-2-09.jpg</t>
   </si>
 </sst>
 </file>
@@ -424,11 +330,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,16 +670,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CE9"/>
+  <dimension ref="A1:CE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="1.140625" customWidth="1"/>
-    <col min="16" max="16" width="166.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="44.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:83" x14ac:dyDescent="0.25">
@@ -825,7 +729,7 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">
@@ -1028,180 +932,6 @@
       </c>
       <c r="CE1" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:83" ht="360" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2">
-        <v>100</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2" t="s">
-        <v>86</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>87</v>
-      </c>
-      <c r="R2" t="s">
-        <v>88</v>
-      </c>
-      <c r="X2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:83" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3">
-        <v>100</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>106</v>
-      </c>
-      <c r="O3" t="s">
-        <v>86</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>87</v>
-      </c>
-      <c r="R3" t="s">
-        <v>88</v>
-      </c>
-      <c r="X3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:83" ht="195" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K4">
-        <v>100</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>107</v>
-      </c>
-      <c r="O4" t="s">
-        <v>86</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>87</v>
-      </c>
-      <c r="R4" t="s">
-        <v>88</v>
-      </c>
-      <c r="X4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>100</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="AZ9">
-        <f>LEN(AZ4)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1219,10 +949,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>